<commit_message>
Act. saud (Estadísticas vitales)
</commit_message>
<xml_diff>
--- a/Data/Ficha educación cambios.xlsx
+++ b/Data/Ficha educación cambios.xlsx
@@ -18,7 +18,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AN$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1046,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>